<commit_message>
Added micro SD so we can get one from lab stores
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Uni\2018-19\D4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA537C4-3AC0-448B-B901-927A134D663A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ABD046-6438-40AD-A2D4-BAE01F72CEA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{848010F5-F588-4E46-9135-8ADA20557D15}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Item</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Batteries</t>
+  </si>
+  <si>
+    <t>micro SD card for Pi</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -144,7 +147,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -625,6 +628,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
         <f t="shared" si="0"/>

</xml_diff>